<commit_message>
Added RNN row and 0/NaN indicator col
</commit_message>
<xml_diff>
--- a/MK/modelIterations.xlsx
+++ b/MK/modelIterations.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e358021\Documents\Berkeley\W207\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F1E7067-4CA2-46B7-B2BA-E020CE0BDB6A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE420F0-7988-4835-82A1-4B75C6DE9723}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modelIterations" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>Season Totals</t>
   </si>
@@ -89,12 +89,15 @@
   </si>
   <si>
     <t>Random Forest</t>
+  </si>
+  <si>
+    <t>RNN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -689,7 +692,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -706,53 +709,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1108,292 +1144,341 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" style="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="16.7109375" style="1"/>
+    <col min="1" max="1" width="16.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="27" customWidth="1"/>
+    <col min="3" max="3" width="2" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="16.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="9" t="s">
+    <row r="1" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="9" t="s">
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="9" t="s">
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="9" t="s">
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="9" t="s">
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="11"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="20"/>
     </row>
-    <row r="2" spans="1:22" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="4" t="s">
+    <row r="2" spans="1:23" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="M2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="N2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="O2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="Q2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="R2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="12" t="s">
+      <c r="U2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="V2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="W2" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="2"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="2"/>
-      <c r="V3" s="3"/>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="2"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="2"/>
+      <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
+    <row r="4" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26"/>
+      <c r="B4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="8"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="8"/>
-      <c r="V4" s="7"/>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="7"/>
+      <c r="W4" s="6"/>
     </row>
-    <row r="5" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7" t="s">
+    <row r="5" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26"/>
+      <c r="B5" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="8"/>
-      <c r="V5" s="7"/>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="7"/>
+      <c r="W5" s="6"/>
     </row>
-    <row r="6" spans="1:22" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16" t="s">
+    <row r="6" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
+      <c r="B6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="17"/>
-      <c r="V6" s="16"/>
+      <c r="C6" s="11">
+        <v>0</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="12"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="12"/>
+      <c r="W6" s="11"/>
     </row>
-    <row r="7" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+    <row r="7" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="19"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="R7" s="20"/>
-      <c r="S7" s="19"/>
-      <c r="V7" s="20"/>
+      <c r="C7" s="15">
+        <v>0</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="14"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="14"/>
+      <c r="W7" s="15"/>
     </row>
-    <row r="8" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+    <row r="8" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="19"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="19"/>
-      <c r="V8" s="20"/>
+      <c r="C8" s="15">
+        <v>0</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="14"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="14"/>
+      <c r="W8" s="15"/>
     </row>
-    <row r="9" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+    <row r="9" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="19"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="19"/>
-      <c r="V9" s="20"/>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="2"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="2"/>
+      <c r="W9" s="3"/>
     </row>
-    <row r="10" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="12"/>
+      <c r="W10" s="11"/>
+    </row>
+    <row r="11" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="2"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="2"/>
-      <c r="V10" s="3"/>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="2"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="2"/>
+      <c r="W11" s="3"/>
     </row>
-    <row r="11" spans="1:22" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16" t="s">
+    <row r="12" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="17"/>
-      <c r="V11" s="16"/>
+      <c r="C12" s="11">
+        <v>0</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="12"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="12"/>
+      <c r="W12" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A10:A11"/>
+  <mergeCells count="8">
+    <mergeCell ref="A11:A12"/>
     <mergeCell ref="A3:A6"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="T1:W1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
functionalization and initial results in spreadsheet
</commit_message>
<xml_diff>
--- a/MK/modelIterations.xlsx
+++ b/MK/modelIterations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrkawa\Documents\Berkeley\w207\fantasyFootballML\MK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e358021\Documents\Berkeley\W207\finalProj\fantasyFootballML-master\MK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2ED33E3-8CA6-4F5E-B5E5-F24A55272E0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F44FAC4-2D5A-4EF9-8674-044309F56805}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modelIterations" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="29">
   <si>
     <t>Split by Position</t>
   </si>
@@ -72,9 +72,6 @@
     <t>SVM</t>
   </si>
   <si>
-    <t>Kernel Ridge</t>
-  </si>
-  <si>
     <t>Neighbors</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>Random Forest</t>
   </si>
   <si>
-    <t>RNN</t>
-  </si>
-  <si>
     <t>Play Mean Data</t>
   </si>
   <si>
@@ -106,6 +100,21 @@
   </si>
   <si>
     <t>Ridge</t>
+  </si>
+  <si>
+    <t>Standardization</t>
+  </si>
+  <si>
+    <t>R^2</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>Kernel Ridge (Linear)</t>
   </si>
 </sst>
 </file>
@@ -628,34 +637,34 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
+      <left style="thin">
         <color indexed="64"/>
-      </top>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -706,7 +715,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -747,15 +756,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -771,38 +771,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1159,132 +1177,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z13"/>
+  <dimension ref="A1:AG32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="18" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15" style="9" customWidth="1"/>
-    <col min="22" max="22" width="4.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15" style="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="16.7109375" style="1"/>
+    <col min="21" max="22" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15" style="9" customWidth="1"/>
+    <col min="28" max="28" width="4.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="4.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="34" max="16384" width="16.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="26" t="s">
+    <row r="1" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="23"/>
+    </row>
+    <row r="2" spans="1:33" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="28"/>
-    </row>
-    <row r="2" spans="1:26" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="4" t="s">
+      <c r="G2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="K2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="P2" s="8" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="R2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="S2" s="4" t="s">
@@ -1294,220 +1319,771 @@
         <v>5</v>
       </c>
       <c r="U2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="V2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="W2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="Y2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="Z2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AB2" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="AC2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG2" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="F3" s="3"/>
-      <c r="K3" s="2"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="2"/>
+      <c r="C3" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2">
+        <v>31.7</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="N3" s="2"/>
+      <c r="R3" s="3"/>
       <c r="S3" s="2"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="2"/>
-      <c r="Z3" s="3"/>
-    </row>
-    <row r="4" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
-      <c r="B4" s="21" t="s">
+      <c r="X3" s="2"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="2"/>
+      <c r="AG3" s="3"/>
+    </row>
+    <row r="4" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="7">
+        <v>47.1</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="N4" s="7"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="7"/>
+      <c r="AG4" s="6"/>
+    </row>
+    <row r="5" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="F4" s="6"/>
-      <c r="K4" s="7"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="7"/>
-      <c r="Z4" s="6"/>
-    </row>
-    <row r="5" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="21" t="s">
+      <c r="D5" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="N5" s="12"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="12"/>
+      <c r="AG5" s="11"/>
+    </row>
+    <row r="6" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="27"/>
+      <c r="B6" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2">
+        <v>31.7</v>
+      </c>
+      <c r="E6" s="10">
+        <v>31.6</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="N6" s="2"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="2"/>
+      <c r="AG6" s="3"/>
+    </row>
+    <row r="7" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="7">
+        <v>47.4</v>
+      </c>
+      <c r="E7" s="9">
+        <v>47.3</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="N7" s="7"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="7"/>
+      <c r="AG7" s="6"/>
+    </row>
+    <row r="8" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0.45</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="N8" s="12"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="12"/>
+      <c r="X8" s="12"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="12"/>
+      <c r="AG8" s="11"/>
+    </row>
+    <row r="9" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="F5" s="6"/>
-      <c r="K5" s="7"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="7"/>
-      <c r="Z5" s="6"/>
-    </row>
-    <row r="6" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
-      <c r="B6" s="21" t="s">
+      <c r="C9" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="2">
+        <v>31.6</v>
+      </c>
+      <c r="E9" s="10">
+        <v>31.8</v>
+      </c>
+      <c r="G9" s="10">
+        <v>31.7</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="N9" s="2"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="2"/>
+      <c r="AG9" s="3"/>
+    </row>
+    <row r="10" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="7">
+        <v>47.3</v>
+      </c>
+      <c r="E10" s="9">
+        <v>47.4</v>
+      </c>
+      <c r="G10" s="9">
+        <v>47.4</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="N10" s="7"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="7"/>
+      <c r="AG10" s="6"/>
+    </row>
+    <row r="11" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0.45</v>
+      </c>
+      <c r="G11" s="13">
+        <v>0.45</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="N11" s="12"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="12"/>
+      <c r="AG11" s="11"/>
+    </row>
+    <row r="12" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27"/>
+      <c r="B12" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="F6" s="6"/>
-      <c r="K6" s="7"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="7"/>
-      <c r="Z6" s="6"/>
-    </row>
-    <row r="7" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="22" t="s">
+      <c r="C12" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="2">
+        <v>31.6</v>
+      </c>
+      <c r="E12" s="10">
+        <v>31.6</v>
+      </c>
+      <c r="G12" s="10">
+        <v>31.7</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="N12" s="2"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="2"/>
+      <c r="AG12" s="3"/>
+    </row>
+    <row r="13" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="7">
+        <v>47.3</v>
+      </c>
+      <c r="E13" s="9">
+        <v>47.3</v>
+      </c>
+      <c r="G13" s="9">
+        <v>47.4</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="N13" s="7"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="AB13" s="6"/>
+      <c r="AC13" s="7"/>
+      <c r="AG13" s="6"/>
+    </row>
+    <row r="14" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0.45</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0.45</v>
+      </c>
+      <c r="H14" s="11"/>
+      <c r="N14" s="12"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="12"/>
+      <c r="X14" s="12"/>
+      <c r="AB14" s="11"/>
+      <c r="AC14" s="12"/>
+      <c r="AG14" s="11"/>
+    </row>
+    <row r="15" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
+      <c r="B15" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="F7" s="11"/>
-      <c r="K7" s="12"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="12"/>
-      <c r="Z7" s="11"/>
-    </row>
-    <row r="8" spans="1:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="C15" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="2">
+        <v>31.6</v>
+      </c>
+      <c r="E15" s="10">
+        <v>31.6</v>
+      </c>
+      <c r="G15" s="10">
+        <v>31.7</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="N15" s="2"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="2"/>
+      <c r="AG15" s="3"/>
+    </row>
+    <row r="16" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="7">
+        <v>47.3</v>
+      </c>
+      <c r="E16" s="9">
+        <v>47.3</v>
+      </c>
+      <c r="G16" s="9">
+        <v>47.4</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="N16" s="7"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="7"/>
+      <c r="AG16" s="6"/>
+    </row>
+    <row r="17" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="E17" s="13">
+        <v>0.45</v>
+      </c>
+      <c r="G17" s="13">
+        <v>0.45</v>
+      </c>
+      <c r="H17" s="11"/>
+      <c r="N17" s="12"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="12"/>
+      <c r="X17" s="12"/>
+      <c r="AB17" s="11"/>
+      <c r="AC17" s="12"/>
+      <c r="AG17" s="11"/>
+    </row>
+    <row r="18" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B18" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="7">
+        <v>29.9</v>
+      </c>
+      <c r="E18" s="9">
+        <v>29.9</v>
+      </c>
+      <c r="G18" s="9">
+        <v>29.7</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="N18" s="7"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="7"/>
+      <c r="AG18" s="6"/>
+    </row>
+    <row r="19" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="27"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="7">
+        <v>50.4</v>
+      </c>
+      <c r="E19" s="9">
+        <v>50.3</v>
+      </c>
+      <c r="G19" s="9">
+        <v>50.2</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="N19" s="7"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="AB19" s="6"/>
+      <c r="AC19" s="7"/>
+      <c r="AG19" s="6"/>
+    </row>
+    <row r="20" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="28"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="12">
+        <v>0.38</v>
+      </c>
+      <c r="E20" s="13">
+        <v>0.38</v>
+      </c>
+      <c r="G20" s="13">
+        <v>0.38</v>
+      </c>
+      <c r="H20" s="11"/>
+      <c r="N20" s="12"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="12"/>
+      <c r="X20" s="12"/>
+      <c r="AB20" s="11"/>
+      <c r="AC20" s="12"/>
+      <c r="AG20" s="11"/>
+    </row>
+    <row r="21" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="F8" s="15"/>
-      <c r="K8" s="14"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="14"/>
-      <c r="Z8" s="15"/>
-    </row>
-    <row r="9" spans="1:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="B21" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="C21" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="2">
+        <v>33.1</v>
+      </c>
+      <c r="E21" s="10">
+        <v>31.6</v>
+      </c>
+      <c r="G21" s="10">
+        <v>30.4</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="N21" s="2"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="2"/>
+      <c r="AG21" s="3"/>
+    </row>
+    <row r="22" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="7">
+        <v>48.8</v>
+      </c>
+      <c r="E22" s="9">
+        <v>47.7</v>
+      </c>
+      <c r="G22" s="9">
+        <v>47</v>
+      </c>
+      <c r="H22" s="6"/>
+      <c r="N22" s="7"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="7"/>
+      <c r="X22" s="7"/>
+      <c r="AB22" s="6"/>
+      <c r="AC22" s="7"/>
+      <c r="AG22" s="6"/>
+    </row>
+    <row r="23" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="28"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="12">
+        <v>0.41</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0.45</v>
+      </c>
+      <c r="G23" s="13">
+        <v>0.46</v>
+      </c>
+      <c r="H23" s="11"/>
+      <c r="N23" s="12"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="12"/>
+      <c r="X23" s="12"/>
+      <c r="AB23" s="11"/>
+      <c r="AC23" s="12"/>
+      <c r="AG23" s="11"/>
+    </row>
+    <row r="24" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="F9" s="15"/>
-      <c r="K9" s="14"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="14"/>
-      <c r="Z9" s="15"/>
-    </row>
-    <row r="10" spans="1:26" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="B24" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="C24" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="2">
+        <v>29.7</v>
+      </c>
+      <c r="H24" s="3"/>
+      <c r="N24" s="2"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="AB24" s="3"/>
+      <c r="AC24" s="2"/>
+      <c r="AG24" s="3"/>
+    </row>
+    <row r="25" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="27"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="7">
+        <v>49.5</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="N25" s="7"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="7"/>
+      <c r="X25" s="7"/>
+      <c r="AB25" s="6"/>
+      <c r="AC25" s="7"/>
+      <c r="AG25" s="6"/>
+    </row>
+    <row r="26" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="28"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="H26" s="11"/>
+      <c r="N26" s="12"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="12"/>
+      <c r="X26" s="12"/>
+      <c r="AB26" s="11"/>
+      <c r="AC26" s="12"/>
+      <c r="AG26" s="11"/>
+    </row>
+    <row r="27" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="F10" s="3"/>
-      <c r="K10" s="2"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="2"/>
-      <c r="Z10" s="3"/>
-    </row>
-    <row r="11" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="F11" s="11"/>
-      <c r="K11" s="12"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="12"/>
-      <c r="S11" s="12"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="12"/>
-      <c r="Z11" s="11"/>
-    </row>
-    <row r="12" spans="1:26" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="B27" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="C27" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="H27" s="3"/>
+      <c r="N27" s="2"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="AB27" s="3"/>
+      <c r="AC27" s="2"/>
+      <c r="AG27" s="3"/>
+    </row>
+    <row r="28" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="30"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="H28" s="6"/>
+      <c r="N28" s="7"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="7"/>
+      <c r="X28" s="7"/>
+      <c r="AB28" s="6"/>
+      <c r="AC28" s="7"/>
+      <c r="AG28" s="6"/>
+    </row>
+    <row r="29" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="30"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="12"/>
+      <c r="H29" s="11"/>
+      <c r="N29" s="12"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="12"/>
+      <c r="X29" s="12"/>
+      <c r="AB29" s="11"/>
+      <c r="AC29" s="12"/>
+      <c r="AG29" s="11"/>
+    </row>
+    <row r="30" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="30"/>
+      <c r="B30" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="F12" s="3"/>
-      <c r="K12" s="2"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="V12" s="3"/>
-      <c r="W12" s="2"/>
-      <c r="Z12" s="3"/>
-    </row>
-    <row r="13" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="F13" s="11"/>
-      <c r="K13" s="12"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="12"/>
-      <c r="S13" s="12"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="12"/>
-      <c r="Z13" s="11"/>
+      <c r="C30" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="H30" s="6"/>
+      <c r="N30" s="7"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="7"/>
+      <c r="X30" s="7"/>
+      <c r="AB30" s="6"/>
+      <c r="AC30" s="7"/>
+      <c r="AG30" s="6"/>
+    </row>
+    <row r="31" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="30"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="H31" s="6"/>
+      <c r="N31" s="7"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="7"/>
+      <c r="X31" s="7"/>
+      <c r="AB31" s="6"/>
+      <c r="AC31" s="7"/>
+      <c r="AG31" s="6"/>
+    </row>
+    <row r="32" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="31"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="12"/>
+      <c r="H32" s="11"/>
+      <c r="N32" s="12"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="12"/>
+      <c r="X32" s="12"/>
+      <c r="AB32" s="11"/>
+      <c r="AC32" s="12"/>
+      <c r="AG32" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="W1:Z1"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="G1:J1"/>
+  <mergeCells count="21">
+    <mergeCell ref="A3:A17"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="AC1:AG1"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="X1:AB1"/>
+    <mergeCell ref="S1:W1"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B21:B23"/>
   </mergeCells>
+  <conditionalFormatting sqref="A3:XFD3 A6:XFD6 A9:XFD9 A12:XFD12 A18:XFD18 A15:XFD15 A21:XFD21 A24:XFD24 A27:XFD27 A30:XFD30">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:XFD4 A7:XFD7 A10:XFD10 A13:XFD13 A16:XFD16 A19:XFD19 A22:XFD22 A25:XFD25 A28:XFD28 A31:XFD31">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32:XFD32 A29:XFD29 A26:XFD26 A23:XFD23 A20:XFD20 A17:XFD17 A14:XFD14 A11:XFD11 A8:XFD8 A5:XFD5">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;C_x000D__x000D_</oddHeader>
-    <oddFooter>&amp;C_x000D__x000D_</oddFooter>
-    <evenHeader>&amp;C_x000D__x000D_</evenHeader>
-    <evenFooter>&amp;C_x000D__x000D_</evenFooter>
-    <firstHeader>&amp;C_x000D__x000D_</firstHeader>
-    <firstFooter>&amp;C_x000D__x000D_</firstFooter>
+    <oddHeader>&amp;C_x000D__x000D__x000D_</oddHeader>
+    <oddFooter>&amp;C_x000D__x000D__x000D_</oddFooter>
+    <evenHeader>&amp;C_x000D__x000D__x000D_</evenHeader>
+    <evenFooter>&amp;C_x000D__x000D__x000D_</evenFooter>
+    <firstHeader>&amp;C_x000D__x000D__x000D_</firstHeader>
+    <firstFooter>&amp;C_x000D__x000D__x000D_</firstFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>